<commit_message>
Update prediction file: Github_Prediction_Storage/predictions.xlsx
</commit_message>
<xml_diff>
--- a/Github_Prediction_Storage/predictions.xlsx
+++ b/Github_Prediction_Storage/predictions.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>bill_length_mm</t>
   </si>
@@ -43,22 +43,31 @@
     <t>39.1</t>
   </si>
   <si>
-    <t>210.5</t>
-  </si>
-  <si>
-    <t>0.45</t>
+    <t>46.5</t>
+  </si>
+  <si>
+    <t>181.0</t>
+  </si>
+  <si>
+    <t>192.0</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>0.09</t>
   </si>
   <si>
     <t>0.0</t>
   </si>
   <si>
-    <t>0.55</t>
+    <t>0.91</t>
   </si>
   <si>
     <t>v1.0</t>
   </si>
   <si>
-    <t>2025-05-04 20:20:51</t>
+    <t>2025-05-04 20:32:52</t>
   </si>
 </sst>
 </file>
@@ -416,7 +425,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -453,25 +462,51 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
         <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>